<commit_message>
Fix test plan notification tool link
</commit_message>
<xml_diff>
--- a/scripts/codemagic-ci/testing/PR-Test-Plan-Template-iOS-QA.xlsx
+++ b/scripts/codemagic-ci/testing/PR-Test-Plan-Template-iOS-QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbryant/Downloads/tps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbryant/UCSD/campusmobile/scripts/codemagic-ci/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E03FDB-FCBC-614B-AD81-752D205A555D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3D6370-9E6F-9546-9E3F-B770E3449134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1200" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PR Test Plan" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -408,10 +408,10 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -420,10 +420,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -438,40 +438,10 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -481,6 +451,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1019,10 +992,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="16"/>
@@ -1043,14 +1016,14 @@
       <c r="U3" s="16"/>
     </row>
     <row r="4" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="D4" s="31" t="s">
+      <c r="B4" s="8"/>
+      <c r="D4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="16"/>
@@ -1071,14 +1044,14 @@
       <c r="U4" s="16"/>
     </row>
     <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="D5" s="27" t="s">
+      <c r="B5" s="8"/>
+      <c r="D5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="16"/>
@@ -1099,14 +1072,14 @@
       <c r="U5" s="16"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="D6" s="27" t="s">
+      <c r="B6" s="8"/>
+      <c r="D6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="16"/>
@@ -1127,12 +1100,12 @@
       <c r="U6" s="16"/>
     </row>
     <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="8"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1151,10 +1124,10 @@
       <c r="U7" s="16"/>
     </row>
     <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="8"/>
       <c r="D8" s="23" t="s">
         <v>17</v>
       </c>
@@ -1177,10 +1150,10 @@
       <c r="U8" s="16"/>
     </row>
     <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="14"/>
@@ -1206,7 +1179,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="22" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="15"/>
@@ -1228,11 +1201,11 @@
       <c r="U10" s="16"/>
     </row>
     <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="D11" s="27" t="s">
+      <c r="B11" s="8"/>
+      <c r="D11" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="18"/>
@@ -1254,12 +1227,12 @@
       <c r="U11" s="16"/>
     </row>
     <row r="12" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="19"/>
@@ -1286,8 +1259,8 @@
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
@@ -1306,10 +1279,10 @@
       <c r="U13" s="16"/>
     </row>
     <row r="14" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="22"/>
       <c r="D14" s="25" t="s">
         <v>28</v>
@@ -1333,15 +1306,15 @@
       <c r="U14" s="16"/>
     </row>
     <row r="15" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="22"/>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
@@ -1365,10 +1338,10 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="22"/>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
@@ -1387,10 +1360,9 @@
       <c r="U16" s="16"/>
     </row>
     <row r="17" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="27" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="24"/>
@@ -1404,13 +1376,11 @@
       <c r="M17" s="16"/>
     </row>
     <row r="18" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26"/>
-      <c r="B18" s="34"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="28"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
@@ -1429,13 +1399,11 @@
       <c r="U18" s="16"/>
     </row>
     <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26"/>
-      <c r="B19" s="34"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="28"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
@@ -1454,13 +1422,11 @@
       <c r="U19" s="16"/>
     </row>
     <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="26"/>
-      <c r="B20" s="34"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="28"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
@@ -1479,10 +1445,8 @@
       <c r="U20" s="16"/>
     </row>
     <row r="21" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="26"/>
-      <c r="B21" s="34"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="27" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="16"/>
@@ -22812,6 +22776,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5D778AC6A79A84EAA5B25C5A2BFF7B6" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4061397ea8fd8f272d8b26ba942e61d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cd0eaed-44fe-4f97-8632-c05a782ebbb7" xmlns:ns3="75164c79-2692-43d6-94a7-34b44bf80abd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b13378bff9c1c8ba474ff50185c4976f" ns2:_="" ns3:_="">
     <xsd:import namespace="3cd0eaed-44fe-4f97-8632-c05a782ebbb7"/>
@@ -22976,12 +22946,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -22992,6 +22956,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D8340-318B-43DD-BE9C-C876AB21B0D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55915E3D-8D32-4904-AE11-02FF4B35B651}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23010,15 +22983,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D8340-318B-43DD-BE9C-C876AB21B0D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{075245DD-0B21-42AF-837E-557C93B33EF5}">
   <ds:schemaRefs>

</xml_diff>